<commit_message>
HOD Content Sent out checked in
HOD Content Sent out checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/Inspiree/HOD-Content-Sendout-Info.xlsx
+++ b/Offline/BusinessManagement/Information/Inspiree/HOD-Content-Sendout-Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Inspiree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D8E973-8A83-4212-9E0C-C59601762BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9123E2EE-9920-474F-BA6B-C04EE98D6EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -488,7 +488,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,6 +598,9 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>9674569343</v>
+      </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
@@ -636,6 +639,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>9830304429</v>
+      </c>
       <c r="G13" s="3" t="s">
         <v>29</v>
       </c>
@@ -655,6 +661,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>9836581909</v>
+      </c>
       <c r="G16" s="3" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Debolina Sen offer letter done
Debolina Sen offer letter done
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/Inspiree/HOD-Content-Sendout-Info.xlsx
+++ b/Offline/BusinessManagement/Information/Inspiree/HOD-Content-Sendout-Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Inspiree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9123E2EE-9920-474F-BA6B-C04EE98D6EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AFF945-A127-42A8-819D-B6960C6FFDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -488,7 +488,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Offer letter of Subrata Ghosh done
Offer letter of Subrata Ghosh done
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/Inspiree/HOD-Content-Sendout-Info.xlsx
+++ b/Offline/BusinessManagement/Information/Inspiree/HOD-Content-Sendout-Info.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Inspiree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AFF945-A127-42A8-819D-B6960C6FFDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD7276-A3FE-4AE8-B8F9-08B4CCC481D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>SlNo</t>
   </si>
@@ -139,13 +140,16 @@
   </si>
   <si>
     <t>https://drive.google.com/drive/folders/12eUnWi0f9Iqb2Un-hgWtxxACOiB7BcIp</t>
+  </si>
+  <si>
+    <t>Science 12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +169,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -204,6 +215,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -487,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,4 +697,77 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE91033-1218-485A-A626-71CCE9682D7C}">
+  <dimension ref="G5:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="71.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G6" r:id="rId1" xr:uid="{C0896806-E565-47EC-9D92-26692164D9A1}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{00841763-E7ED-4715-BFDE-C0857968F0F8}"/>
+    <hyperlink ref="G12" r:id="rId3" xr:uid="{B8CFD8E9-4BB5-4BBF-B444-35CFFEEB4BB0}"/>
+    <hyperlink ref="G15" r:id="rId4" xr:uid="{8F3AD4F7-27C9-4891-9FA5-38270CF09113}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Anupam Sen contact details stored
Anupam Sen contact details stored
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/Inspiree/HOD-Content-Sendout-Info.xlsx
+++ b/Offline/BusinessManagement/Information/Inspiree/HOD-Content-Sendout-Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Inspiree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD7276-A3FE-4AE8-B8F9-08B4CCC481D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7C08B3-CEE5-439B-AA68-9FF0682D9155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE91033-1218-485A-A626-71CCE9682D7C}">
   <dimension ref="G5:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>